<commit_message>
restructure files, first drafts of design docs
</commit_message>
<xml_diff>
--- a/_3 Develop/Component Data-Info/Interface PCB/IO Calculations.xlsx
+++ b/_3 Develop/Component Data-Info/Interface PCB/IO Calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\OLS Level Test Project\_Component Data-Info\Interface PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AllenProjects\PM_Folder\_3 Develop\Component Data-Info\Interface PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFF501C-439C-451D-A185-EE42C4F409B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFBCA8D-3083-4356-9E62-C23BB1E5E1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26565" yWindow="1065" windowWidth="23700" windowHeight="13770" xr2:uid="{354FACC5-74DC-4F63-AF62-72750756D9DC}"/>
+    <workbookView xWindow="1180" yWindow="740" windowWidth="17550" windowHeight="11280" xr2:uid="{354FACC5-74DC-4F63-AF62-72750756D9DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Iref &amp; Ain " sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>LT3092</t>
   </si>
@@ -104,10 +104,28 @@
     <t>diff</t>
   </si>
   <si>
-    <t>Iref ma</t>
-  </si>
-  <si>
     <t xml:space="preserve">                </t>
+  </si>
+  <si>
+    <t>Iout ma</t>
+  </si>
+  <si>
+    <t>Vc</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>Rdut</t>
+  </si>
+  <si>
+    <t>Voff</t>
   </si>
 </sst>
 </file>
@@ -165,7 +183,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -181,6 +199,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -319,13 +338,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>36870</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>36417</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -363,13 +382,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>533382</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>156546</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -753,24 +772,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{167A66C8-747A-4DA5-AC59-C33924118364}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -778,15 +797,15 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1.4E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.47E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -794,16 +813,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="6">
         <f>B3*B4/B2</f>
-        <v>20999.999999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22050</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -811,16 +830,16 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4">
         <f>B6*B2/B4*1000</f>
         <v>14.666666666666668</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -828,149 +847,202 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <f>B9-B7*B4/1000</f>
+        <v>23.78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="8">
-        <f>B9/B7*1000</f>
-        <v>1636.3636363636363</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" s="8">
+        <f>B10/B7*1000</f>
+        <v>1621.3636363636363</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B12" s="8">
         <v>1400</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="9">
-        <f>B7*B11/1000</f>
-        <v>20.533333333333335</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="9">
+        <f>B7*B12/1000</f>
+        <v>20.533333333333335</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="9">
         <f>10</f>
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="2">
-        <f>B13/B12</f>
+      <c r="B15" s="2">
+        <f>B14/B13</f>
         <v>0.48701298701298695</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B19" s="11">
         <v>1000000</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="8">
-        <v>110000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" s="8">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="10">
-        <f>B18*B19/(B18+B19)</f>
-        <v>99099.099099099098</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" s="10">
+        <f>B19*B20/(B19+B20)</f>
+        <v>909090.90909090906</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="10">
-        <f>(B20-B14*B20)/B14</f>
-        <v>104384.38438438441</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" s="10">
+        <f>(B21-B15*B21)/B15</f>
+        <v>957575.75757575769</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="10">
-        <f>B19+B21</f>
-        <v>214384.38438438441</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="B23" s="10">
+        <f>B20+B22</f>
+        <v>10957575.757575758</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="11">
-        <v>104700</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B24" s="11">
+        <v>950000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>1100</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>20</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="1">
-        <f>$B$22/($B$22+B25)*$B$7</f>
-        <v>14.591796585572743</v>
-      </c>
-      <c r="M27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" s="1">
+        <f>$B$23/($B$23+B26)*$B$7</f>
+        <v>14.665194469323646</v>
+      </c>
+      <c r="M28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="1">
-        <f>$B$22/($B$22+B26)*$B$7</f>
-        <v>14.659828562014544</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" s="1">
+        <f>$B$23/($B$23+B27)*$B$7</f>
+        <v>14.66653281833066</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="12">
-        <f>(B27-B28)/B27</f>
-        <v>-4.6623440809931815E-3</v>
-      </c>
+      <c r="B30" s="12">
+        <f>(B28-B29)/B28</f>
+        <v>-9.1260229096419275E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="13">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="13">
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="13">
+        <f>0.0147*E33*E35/(E34+E35)+B31</f>
+        <v>0.89750000000000008</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="E37" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -987,15 +1059,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B529C28E597C4644883DFF02F5439745" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8abda5ff0f70db93971ebd3374971fd9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ee70e6cf-5544-46a7-8a87-c33a81038da8" xmlns:ns4="c34b6e8a-d710-43c6-a1e4-4b960193726d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff1ae8cf5eb2bc1782f971886c50b8c8" ns3:_="" ns4:_="">
     <xsd:import namespace="ee70e6cf-5544-46a7-8a87-c33a81038da8"/>
@@ -1216,6 +1279,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B6F8E6C-B1B4-4BAE-83DE-D70A997974BC}">
   <ds:schemaRefs>
@@ -1234,14 +1306,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D85756E-0C5A-4F42-B521-0E8F1844F349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A81CDC90-40E4-4A27-82DD-02E5ECB3DC67}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1258,4 +1322,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D85756E-0C5A-4F42-B521-0E8F1844F349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>